<commit_message>
Before refactoring the ExportOutstandingDuesToExcel to a private method in order encapsulate only the core functionality in to a separate method and only the basic steps of creating the Workbook remains in the main method which can later be moved to some other class conveniently.
</commit_message>
<xml_diff>
--- a/SlvParkview.FinanceManager/SlvParkview.FinanceManager/Move to Bin/Data Format.xlsx
+++ b/SlvParkview.FinanceManager/SlvParkview.FinanceManager/Move to Bin/Data Format.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masanams\source\SriniHomePracticeRepos\SlvParkview.FinanceManager\SlvParkview.FinanceManager\Move to Bin\"/>
@@ -420,10 +420,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,6 +459,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Random data is added to Data Format excel file and some logic for exporting from Excel to Json is added.
</commit_message>
<xml_diff>
--- a/SlvParkview.FinanceManager/SlvParkview.FinanceManager/Move to Bin/Data Format.xlsx
+++ b/SlvParkview.FinanceManager/SlvParkview.FinanceManager/Move to Bin/Data Format.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masanams\source\SriniHomePracticeRepos\SlvParkview.FinanceManager\SlvParkview.FinanceManager\Move to Bin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srini\source\repos\SlvParkview.FinanceManager\SlvParkview.FinanceManager\Move to Bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAFB2CB-82E1-4218-B011-82F78FBA2779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14250"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block Details" sheetId="1" r:id="rId1"/>
     <sheet name="Payments History" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Flat No.</t>
   </si>
@@ -66,15 +78,63 @@
   <si>
     <t>Tenant Name</t>
   </si>
+  <si>
+    <t>A001</t>
+  </si>
+  <si>
+    <t>A002</t>
+  </si>
+  <si>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>A004</t>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>A006</t>
+  </si>
+  <si>
+    <t>A007</t>
+  </si>
+  <si>
+    <t>A008</t>
+  </si>
+  <si>
+    <t>A101</t>
+  </si>
+  <si>
+    <t>A102</t>
+  </si>
+  <si>
+    <t>A103</t>
+  </si>
+  <si>
+    <t>A104</t>
+  </si>
+  <si>
+    <t>A105</t>
+  </si>
+  <si>
+    <t>A106</t>
+  </si>
+  <si>
+    <t>A107</t>
+  </si>
+  <si>
+    <t>A108</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +155,12 @@
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -419,12 +485,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,14 +517,243 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="str">
+        <f>"Owner Name "&amp;A2</f>
+        <v>Owner Name A001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="str">
+        <f t="shared" ref="B3:B17" si="0">"Owner Name "&amp;A3</f>
+        <v>Owner Name A002</v>
+      </c>
+      <c r="C3" s="6" t="str">
+        <f>"Co-owner Name "&amp;A3</f>
+        <v>Co-owner Name A002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A003</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A004</v>
+      </c>
+      <c r="D5" s="6" t="str">
+        <f>"Tenant Name "&amp;A3</f>
+        <v>Tenant Name A002</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A005</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A006</v>
+      </c>
+      <c r="C7" s="6" t="str">
+        <f>"Co-owner Name "&amp;A7</f>
+        <v>Co-owner Name A006</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A007</v>
+      </c>
+      <c r="D8" s="6" t="str">
+        <f>"Tenant Name "&amp;A6</f>
+        <v>Tenant Name A005</v>
+      </c>
+      <c r="E8" s="2">
+        <v>9650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A008</v>
+      </c>
+      <c r="D9" s="6" t="str">
+        <f>"Tenant Name "&amp;A7</f>
+        <v>Tenant Name A006</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A101</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A102</v>
+      </c>
+      <c r="C11" s="6" t="str">
+        <f>"Co-owner Name "&amp;A11</f>
+        <v>Co-owner Name A102</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A103</v>
+      </c>
+      <c r="D12" s="6" t="str">
+        <f>"Tenant Name "&amp;A10</f>
+        <v>Tenant Name A101</v>
+      </c>
+      <c r="E12" s="2">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A104</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A105</v>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f>"Tenant Name "&amp;A12</f>
+        <v>Tenant Name A103</v>
+      </c>
+      <c r="E14" s="2">
+        <v>22600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A106</v>
+      </c>
+      <c r="C15" s="6" t="str">
+        <f>"Co-owner Name "&amp;A15</f>
+        <v>Co-owner Name A106</v>
+      </c>
+      <c r="E15" s="2">
+        <v>18500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A107</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Owner Name A108</v>
+      </c>
+      <c r="E17" s="2">
+        <v>20450</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>